<commit_message>
update page theme, used bootstrap3.
</commit_message>
<xml_diff>
--- a/databaseDesign/heroku_blog_datebase_v01.xlsx
+++ b/databaseDesign/heroku_blog_datebase_v01.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="572" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="572" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="关系总图" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="115">
   <si>
     <t>数据库关系图：</t>
   </si>
@@ -367,12 +367,60 @@
   <si>
     <t>类型是否可见</t>
   </si>
+  <si>
+    <t>root_id</t>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>是</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>顶级父评论</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="DejaVu Sans"/>
+        <family val="2"/>
+      </rPr>
+      <t>ID</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>，关联自身表的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="DejaVu Sans"/>
+        <family val="2"/>
+      </rPr>
+      <t>ID</t>
+    </r>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="8">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="DejaVu Sans"/>
@@ -420,6 +468,18 @@
       <color theme="10"/>
       <name val="DejaVu Sans"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="6">
@@ -485,7 +545,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -510,10 +570,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -632,14 +693,14 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="CCE8CF"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -930,6 +991,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <headerFooter>
@@ -1028,6 +1090,7 @@
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>
   </mergeCells>
+  <phoneticPr fontId="8" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="A3" location="users!A1" display="users"/>
     <hyperlink ref="A4" location="blog_infos!A1" display="blog_infos"/>
@@ -1222,6 +1285,7 @@
   <mergeCells count="1">
     <mergeCell ref="A1:F1"/>
   </mergeCells>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"DejaVu Serif,Book"&amp;12&amp;A</oddHeader>
@@ -1387,6 +1451,7 @@
   <mergeCells count="1">
     <mergeCell ref="A1:F1"/>
   </mergeCells>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"DejaVu Serif,Book"&amp;12&amp;A</oddHeader>
@@ -1634,6 +1699,7 @@
   <mergeCells count="1">
     <mergeCell ref="A1:F1"/>
   </mergeCells>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"DejaVu Serif,Book"&amp;12&amp;A</oddHeader>
@@ -1646,7 +1712,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
@@ -1766,6 +1832,7 @@
   <mergeCells count="1">
     <mergeCell ref="A1:F1"/>
   </mergeCells>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"DejaVu Serif,Book"&amp;12&amp;A</oddHeader>
@@ -1776,10 +1843,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1915,22 +1982,39 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="10" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B10" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C10" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:F1"/>
   </mergeCells>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter>
@@ -2066,6 +2150,7 @@
   <mergeCells count="1">
     <mergeCell ref="A1:F1"/>
   </mergeCells>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"DejaVu Serif,Book"&amp;12&amp;A</oddHeader>
@@ -2214,6 +2299,8 @@
   <mergeCells count="1">
     <mergeCell ref="A1:F1"/>
   </mergeCells>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>